<commit_message>
Updated 9/10/2017 PVR Tasks
</commit_message>
<xml_diff>
--- a/Sprint_Planning_Document.xlsx
+++ b/Sprint_Planning_Document.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7470" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="7470" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="OMS Backlog" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="183">
   <si>
     <t>Order Management System Sprint Planning Document</t>
   </si>
@@ -755,6 +755,9 @@
   </si>
   <si>
     <t>Mongo Team</t>
+  </si>
+  <si>
+    <t>OMS-0020</t>
   </si>
 </sst>
 </file>
@@ -898,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -986,6 +989,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1302,8 +1308,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C41" sqref="A39:C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,7 +2017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13:C13"/>
     </sheetView>
   </sheetViews>
@@ -2161,10 +2167,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F86"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2789,49 +2795,76 @@
         <v>42896</v>
       </c>
     </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>121</v>
+      </c>
+      <c r="C40" t="s">
+        <v>174</v>
+      </c>
+      <c r="D40" s="43">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>175</v>
+      </c>
+      <c r="D41" s="43">
+        <v>1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>74</v>
+      <c r="A43" s="13">
+        <v>42988</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="C44" t="s">
-        <v>177</v>
+        <v>11</v>
       </c>
       <c r="D44" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C45" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="6"/>
+      <c r="B45" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="6">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D46" s="6">
         <v>2</v>
@@ -2841,37 +2874,116 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C47" s="4" t="s">
-        <v>56</v>
+      <c r="B47" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="6">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
+        <v>182</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="6">
+        <v>1</v>
+      </c>
+      <c r="E48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>111</v>
+      </c>
+      <c r="C80" t="s">
+        <v>177</v>
+      </c>
+      <c r="D80" s="6">
+        <v>2</v>
+      </c>
+      <c r="E80" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C81" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D81" s="6"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="6">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C83" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
         <v>124</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C84" t="s">
         <v>54</v>
       </c>
-      <c r="D48" s="6">
-        <v>2</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="D84" s="6">
+        <v>2</v>
+      </c>
+      <c r="E84" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C49" s="4" t="s">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C85" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>115</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C86" t="s">
         <v>9</v>
       </c>
-      <c r="D50" s="6">
+      <c r="D86" s="6">
         <v>1</v>
       </c>
     </row>
@@ -2885,8 +2997,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G124"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView topLeftCell="A73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>